<commit_message>
Updated with RoHS Compliance Information
Added RoHS References for FAB-ASSY Process
</commit_message>
<xml_diff>
--- a/RoHS Compliance/BD9G341EFJ-E2EVK-101_BOM_REV01_2014-10-17.xlsx
+++ b/RoHS Compliance/BD9G341EFJ-E2EVK-101_BOM_REV01_2014-10-17.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamara\Projects Satya\BD9G341\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbahar\Documents\GitHub\BD9G341AEFJ-EVK-101\RoHS Compliance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="125">
   <si>
     <t>Item</t>
   </si>
@@ -388,13 +388,19 @@
   </si>
   <si>
     <t>TE_RoHS.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAB/ASSY RoHS Certificate of Compliance: </t>
+  </si>
+  <si>
+    <t>FAB-9_FAB-ASSY_RoHS Cert.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +556,15 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF1536DD"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -919,7 +934,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -950,6 +965,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1092,6 +1113,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1127,6 +1165,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1305,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1369,7 @@
     <col min="1" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="22" style="2" bestFit="1" customWidth="1"/>
@@ -1332,7 +1387,13 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="D1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2126,6 +2187,9 @@
       <c r="M26" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="M15" r:id="rId1"/>
     <hyperlink ref="M16" r:id="rId2"/>

</xml_diff>